<commit_message>
atualização, para falta de faixa etária e atualização de núcleo familiar
</commit_message>
<xml_diff>
--- a/assets/sheets/planilha_gerador_modificado.xlsx
+++ b/assets/sheets/planilha_gerador_modificado.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="planilha_gerador" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="report1722698031287" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'planilha_gerador'!$A$1:$N$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'report1722698031287'!$A$1:$N$30</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -930,30 +930,30 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="22" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="36.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="24.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="36" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="25" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="32.28515625" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="35.28515625" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="36.5703125" bestFit="1" customWidth="1" min="10" max="11"/>
-    <col width="20.28515625" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="20.42578125" bestFit="1" customWidth="1" min="13" max="13"/>
-    <col width="33.140625" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="23" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="20.77734375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="33.77734375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="23" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="34.21875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="24.109375" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="30.6640625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="33.21875" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="17.88671875" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="35.5546875" bestFit="1" customWidth="1" min="10" max="11"/>
+    <col width="19.21875" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="19.5546875" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="31.5546875" bestFit="1" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
+    <row r="1" ht="28.8" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Facilitador do Beneficiário</t>
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="E2" s="3" t="n">
-        <v>249</v>
+        <v>270</v>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
@@ -1091,12 +1091,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>BR060100029</t>
+          <t>BR060100037</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Phablo de Lima Paulo</t>
+          <t>Julio Cesar Oliveira Gomes</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -1105,11 +1105,11 @@
         </is>
       </c>
       <c r="E3" s="3" t="n">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>12-14</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="H3" s="4" t="n">
-        <v>44879</v>
+        <v>44875</v>
       </c>
       <c r="I3" s="4" t="n">
         <v>44872</v>
@@ -1142,15 +1142,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n"/>
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Rose Gomes</t>
+        </is>
+      </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>BR060100031</t>
+          <t>BR060100071</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Arthur Oiveira Nobrega</t>
+          <t>Mariana Pereira Cunha</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -1159,23 +1163,23 @@
         </is>
       </c>
       <c r="E4" s="3" t="n">
-        <v>248</v>
+        <v>269</v>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>15-18</t>
         </is>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>Sabrina Martins</t>
+          <t>Rayla Rodrigues</t>
         </is>
       </c>
       <c r="H4" s="4" t="n">
         <v>44873</v>
       </c>
       <c r="I4" s="4" t="n">
-        <v>44873</v>
+        <v>45225</v>
       </c>
       <c r="J4" s="2" t="n"/>
       <c r="K4" s="5" t="n"/>
@@ -1203,12 +1207,12 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>BR060100037</t>
+          <t>BR060100084</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Julio Cesar Oliveira Gomes</t>
+          <t>Douglas Marcelino da Silva</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -1217,7 +1221,7 @@
         </is>
       </c>
       <c r="E5" s="3" t="n">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
@@ -1230,10 +1234,10 @@
         </is>
       </c>
       <c r="H5" s="4" t="n">
-        <v>44875</v>
+        <v>44915</v>
       </c>
       <c r="I5" s="4" t="n">
-        <v>44872</v>
+        <v>44886</v>
       </c>
       <c r="J5" s="2" t="n"/>
       <c r="K5" s="5" t="n"/>
@@ -1261,12 +1265,12 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>BR060100065</t>
+          <t>BR060100144</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Arthur Felipe Agostinho da Silva</t>
+          <t>José Carlos Gouveia Nunes</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -1275,23 +1279,23 @@
         </is>
       </c>
       <c r="E6" s="3" t="n">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>12-14</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>Rayla Rodrigues</t>
+          <t>Márcia Alencar</t>
         </is>
       </c>
       <c r="H6" s="4" t="n">
-        <v>44875</v>
+        <v>44889</v>
       </c>
       <c r="I6" s="4" t="n">
-        <v>44873</v>
+        <v>44886</v>
       </c>
       <c r="J6" s="2" t="n"/>
       <c r="K6" s="5" t="n"/>
@@ -1319,12 +1323,12 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>BR060100071</t>
+          <t>BR060100173</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Mariana Pereira Cunha</t>
+          <t>Allef Pierry Oliveira Paulino</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -1333,23 +1337,23 @@
         </is>
       </c>
       <c r="E7" s="3" t="n">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>15-18</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Rayla Rodrigues</t>
+          <t>Sabrina Martins</t>
         </is>
       </c>
       <c r="H7" s="4" t="n">
-        <v>44873</v>
+        <v>44886</v>
       </c>
       <c r="I7" s="4" t="n">
-        <v>45225</v>
+        <v>44886</v>
       </c>
       <c r="J7" s="2" t="n"/>
       <c r="K7" s="5" t="n"/>
@@ -1377,12 +1381,12 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>BR060100143</t>
+          <t>BR060100252</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Eduardo Caetano Alves Aciole</t>
+          <t>Eloah Ribeiro Queiroz</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -1391,23 +1395,23 @@
         </is>
       </c>
       <c r="E8" s="3" t="n">
-        <v>249</v>
+        <v>332</v>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>6-8</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>Márcia Alencar</t>
+          <t>Diana Oliveira</t>
         </is>
       </c>
       <c r="H8" s="4" t="n">
-        <v>44872</v>
+        <v>44810</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>45132</v>
+        <v>44755</v>
       </c>
       <c r="J8" s="2" t="n"/>
       <c r="K8" s="5" t="n"/>
@@ -1435,12 +1439,12 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>BR060100144</t>
+          <t>BR060100226</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>José Carlos Gouveia Nunes</t>
+          <t>Julia Grazielly Oliveira Gomes</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
@@ -1449,23 +1453,23 @@
         </is>
       </c>
       <c r="E9" s="3" t="n">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>6-8</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Márcia Alencar</t>
+          <t>Ribaneide Rodrigues</t>
         </is>
       </c>
       <c r="H9" s="4" t="n">
-        <v>44889</v>
+        <v>44861</v>
       </c>
       <c r="I9" s="4" t="n">
-        <v>44886</v>
+        <v>44861</v>
       </c>
       <c r="J9" s="2" t="n"/>
       <c r="K9" s="5" t="n"/>
@@ -1493,12 +1497,12 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>BR060100150</t>
+          <t>BR060100243</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Ester de Sousa Mendes</t>
+          <t>José Bernardes Martins Marinho</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -1507,23 +1511,23 @@
         </is>
       </c>
       <c r="E10" s="3" t="n">
-        <v>246</v>
+        <v>281</v>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>6-8</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>KAROLYNA MACENA</t>
+          <t>Ribaneide Rodrigues</t>
         </is>
       </c>
       <c r="H10" s="4" t="n">
-        <v>44875</v>
+        <v>44861</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>44872</v>
+        <v>44861</v>
       </c>
       <c r="J10" s="2" t="n"/>
       <c r="K10" s="5" t="n"/>
@@ -1551,12 +1555,12 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>BR060100173</t>
+          <t>BR060100244</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Allef Pierry Oliveira Paulino</t>
+          <t>Valentina Figueiredo Carvalho</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -1565,16 +1569,16 @@
         </is>
       </c>
       <c r="E11" s="3" t="n">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>6-8</t>
         </is>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>Sabrina Martins</t>
+          <t>Irisnalda Fernandes da Silva</t>
         </is>
       </c>
       <c r="H11" s="4" t="n">
@@ -1609,12 +1613,12 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>BR060100175</t>
+          <t>BR060100314</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Atom Deus dos Santos Araujo</t>
+          <t>Ana Livya Alcantara Batista</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -1623,23 +1627,23 @@
         </is>
       </c>
       <c r="E12" s="3" t="n">
-        <v>249</v>
+        <v>295</v>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>6-8</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>Sabrina Martins</t>
+          <t>Irisnalda Fernandes da Silva</t>
         </is>
       </c>
       <c r="H12" s="4" t="n">
-        <v>44872</v>
+        <v>44847</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>44872</v>
+        <v>44847</v>
       </c>
       <c r="J12" s="2" t="n"/>
       <c r="K12" s="5" t="n"/>
@@ -1667,37 +1671,37 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>BR060100252</t>
+          <t>BR060100004</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Eloah Ribeiro Queiroz</t>
+          <t>Ryan Pablo Pergentino dos Santos Alves</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Aprovado</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="E13" s="3" t="n">
-        <v>311</v>
+        <v>256</v>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>6-8</t>
+          <t>12-14</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Diana Oliveira</t>
+          <t>Rayla Rodrigues</t>
         </is>
       </c>
       <c r="H13" s="4" t="n">
-        <v>44810</v>
+        <v>44886</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>44755</v>
+        <v>44886</v>
       </c>
       <c r="J13" s="2" t="n"/>
       <c r="K13" s="5" t="n"/>
@@ -1725,37 +1729,37 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>BR060100226</t>
+          <t>BR060100029</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Julia Grazielly Oliveira Gomes</t>
+          <t>Phablo de Lima Paulo</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>Aprovado</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="E14" s="3" t="n">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>6-8</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>Ribaneide Rodrigues</t>
+          <t>Rayla Rodrigues</t>
         </is>
       </c>
       <c r="H14" s="4" t="n">
-        <v>44861</v>
+        <v>44879</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>44861</v>
+        <v>44872</v>
       </c>
       <c r="J14" s="2" t="n"/>
       <c r="K14" s="5" t="n"/>
@@ -1783,25 +1787,25 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>BR060100239</t>
+          <t>BR060100031</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Samuel Oliveira do Nascimento</t>
+          <t>Arthur Oiveira Nobrega</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>Aprovado</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="E15" s="3" t="n">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>6-8</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
@@ -1810,10 +1814,10 @@
         </is>
       </c>
       <c r="H15" s="4" t="n">
-        <v>44872</v>
+        <v>44873</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>44872</v>
+        <v>44873</v>
       </c>
       <c r="J15" s="2" t="n"/>
       <c r="K15" s="5" t="n"/>
@@ -1841,37 +1845,37 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>BR060100243</t>
+          <t>BR060100039</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>José Bernardes Martins Marinho</t>
+          <t>Calebe Martins da Silva</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>Aprovado</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="E16" s="3" t="n">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>6-8</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>Ribaneide Rodrigues</t>
+          <t>Márcia Alencar</t>
         </is>
       </c>
       <c r="H16" s="4" t="n">
-        <v>44861</v>
+        <v>44872</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>44861</v>
+        <v>44872</v>
       </c>
       <c r="J16" s="2" t="n"/>
       <c r="K16" s="5" t="n"/>
@@ -1899,37 +1903,37 @@
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>BR060100244</t>
+          <t>BR060100065</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Valentina Figueiredo Carvalho</t>
+          <t>Arthur Felipe Agostinho da Silva</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>Aprovado</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="E17" s="3" t="n">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>6-8</t>
+          <t>12-14</t>
         </is>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>Irisnalda Fernandes da Silva</t>
+          <t>Rayla Rodrigues</t>
         </is>
       </c>
       <c r="H17" s="4" t="n">
-        <v>44886</v>
+        <v>44875</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>44886</v>
+        <v>44873</v>
       </c>
       <c r="J17" s="2" t="n"/>
       <c r="K17" s="5" t="n"/>
@@ -1957,37 +1961,37 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>BR060100314</t>
+          <t>BR060100143</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Ana Livya Alcantara Batista</t>
+          <t>Eduardo Caetano Alves Aciole</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>Aprovado</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="E18" s="3" t="n">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>6-8</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>Irisnalda Fernandes da Silva</t>
+          <t>Márcia Alencar</t>
         </is>
       </c>
       <c r="H18" s="4" t="n">
-        <v>44847</v>
+        <v>44872</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>44847</v>
+        <v>45132</v>
       </c>
       <c r="J18" s="2" t="n"/>
       <c r="K18" s="5" t="n"/>
@@ -2007,7 +2011,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="30" customHeight="1">
+    <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
           <t>Rose Gomes</t>
@@ -2015,12 +2019,12 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>BR060100004</t>
+          <t>BR060100150</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Ryan Pablo Pergentino dos Santos Alves</t>
+          <t>Ester de Sousa Mendes</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
@@ -2029,23 +2033,23 @@
         </is>
       </c>
       <c r="E19" s="3" t="n">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="F19" s="2" t="inlineStr">
         <is>
-          <t>12-14</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>Rayla Rodrigues</t>
+          <t>KAROLYNA MACENA</t>
         </is>
       </c>
       <c r="H19" s="4" t="n">
-        <v>44886</v>
+        <v>44875</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>44886</v>
+        <v>44872</v>
       </c>
       <c r="J19" s="2" t="n"/>
       <c r="K19" s="5" t="n"/>
@@ -2065,7 +2069,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="45" customHeight="1">
+    <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
           <t>Rose Gomes</t>
@@ -2073,12 +2077,12 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>BR060100013</t>
+          <t>BR060100175</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Pedro Henrique Sousa Pereira dos Santos</t>
+          <t>Atom Deus dos Santos Araujo</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
@@ -2087,34 +2091,26 @@
         </is>
       </c>
       <c r="E20" s="3" t="n">
-        <v>249</v>
+        <v>270</v>
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>12-14</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>Rayla Rodrigues</t>
+          <t>Sabrina Martins</t>
         </is>
       </c>
       <c r="H20" s="4" t="n">
         <v>44872</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>45482</v>
-      </c>
-      <c r="J20" s="2" t="inlineStr">
-        <is>
-          <t>Peso e altura errados/desatualizados</t>
-        </is>
-      </c>
-      <c r="K20" s="5" t="inlineStr">
-        <is>
-          <t>- Olá irmãos, é necessário inserir avaliação de saúde atualizada para atualizar peso e altura.</t>
-        </is>
-      </c>
+        <v>44872</v>
+      </c>
+      <c r="J20" s="2" t="n"/>
+      <c r="K20" s="5" t="n"/>
       <c r="L20" s="2" t="inlineStr">
         <is>
           <t>BR0601</t>
@@ -2131,7 +2127,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="30" customHeight="1">
+    <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
           <t>Rose Gomes</t>
@@ -2139,21 +2135,21 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>BR060100030</t>
+          <t>BR060100170</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Lucas Ryan Trajano de Souza</t>
+          <t>Miguel Nunes Farias</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Aprovado</t>
         </is>
       </c>
       <c r="E21" s="3" t="n">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="F21" s="2" t="inlineStr">
         <is>
@@ -2162,25 +2158,17 @@
       </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
-          <t>KAROLYNA MACENA</t>
+          <t>Sabrina Martins</t>
         </is>
       </c>
       <c r="H21" s="4" t="n">
-        <v>44875</v>
+        <v>44869</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>45482</v>
-      </c>
-      <c r="J21" s="2" t="inlineStr">
-        <is>
-          <t>Informação Educacional</t>
-        </is>
-      </c>
-      <c r="K21" s="5" t="inlineStr">
-        <is>
-          <t>Olá irmãos, é necessário atualizar escolaridade.</t>
-        </is>
-      </c>
+        <v>44869</v>
+      </c>
+      <c r="J21" s="2" t="n"/>
+      <c r="K21" s="5" t="n"/>
       <c r="L21" s="2" t="inlineStr">
         <is>
           <t>BR0601</t>
@@ -2193,7 +2181,7 @@
       </c>
       <c r="N21" s="2" t="inlineStr">
         <is>
-          <t>Sponsored</t>
+          <t>Unsponsored</t>
         </is>
       </c>
     </row>
@@ -2205,30 +2193,30 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>BR060100039</t>
+          <t>BR060100239</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Calebe Martins da Silva</t>
+          <t>Samuel Oliveira do Nascimento</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>Enviado</t>
+          <t>Aprovado</t>
         </is>
       </c>
       <c r="E22" s="3" t="n">
-        <v>249</v>
+        <v>270</v>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>6-8</t>
         </is>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>Márcia Alencar</t>
+          <t>Sabrina Martins</t>
         </is>
       </c>
       <c r="H22" s="4" t="n">
@@ -2251,485 +2239,171 @@
       </c>
       <c r="N22" s="2" t="inlineStr">
         <is>
+          <t>Unsponsored</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>Rose Gomes</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>BR060100318</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>Joao Henrique Rodrigues Monteiro</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>298</v>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>6-8</t>
+        </is>
+      </c>
+      <c r="G23" s="2" t="inlineStr">
+        <is>
+          <t>Irisnalda Fernandes da Silva</t>
+        </is>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>44844</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <v>44844</v>
+      </c>
+      <c r="J23" s="2" t="n"/>
+      <c r="K23" s="5" t="n"/>
+      <c r="L23" s="2" t="inlineStr">
+        <is>
+          <t>BR0601</t>
+        </is>
+      </c>
+      <c r="M23" s="2" t="inlineStr">
+        <is>
+          <t>Vencida (19-23)</t>
+        </is>
+      </c>
+      <c r="N23" s="2" t="inlineStr">
+        <is>
+          <t>Unsponsored</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="43.2" customHeight="1">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Rose Gomes</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>BR060100217</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>Lucas Kaun Fernandes</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>Devolvido à Igreja Parceira</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>382</v>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>6-8</t>
+        </is>
+      </c>
+      <c r="G24" s="2" t="inlineStr">
+        <is>
+          <t>Nayara Oliveira</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="n">
+        <v>44760</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <v>45482</v>
+      </c>
+      <c r="J24" s="2" t="inlineStr">
+        <is>
+          <t>Divergência de idade e grupo etário; Núcleo familiar/Responsável primário</t>
+        </is>
+      </c>
+      <c r="K24" s="5" t="inlineStr">
+        <is>
+          <t>Olá irmãos, é necessário que sejam inseridos os nomes completos no núcleo familiar. Atualizar grupo etario.</t>
+        </is>
+      </c>
+      <c r="L24" s="2" t="inlineStr">
+        <is>
+          <t>BR0601</t>
+        </is>
+      </c>
+      <c r="M24" s="2" t="inlineStr">
+        <is>
+          <t>Muito vencida (&gt;=24)</t>
+        </is>
+      </c>
+      <c r="N24" s="2" t="inlineStr">
+        <is>
           <t>Sponsored</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="60" customHeight="1">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>Rose Gomes</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="inlineStr">
-        <is>
-          <t>BR060100172</t>
-        </is>
-      </c>
-      <c r="C23" s="2" t="inlineStr">
-        <is>
-          <t>Miguel Dhuart de Lima Paulo</t>
-        </is>
-      </c>
-      <c r="D23" s="2" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E23" s="3" t="n">
-        <v>245</v>
-      </c>
-      <c r="F23" s="2" t="inlineStr">
-        <is>
-          <t>9-11</t>
-        </is>
-      </c>
-      <c r="G23" s="2" t="inlineStr">
-        <is>
-          <t>Sabrina Martins</t>
-        </is>
-      </c>
-      <c r="H23" s="4" t="n">
-        <v>44876</v>
-      </c>
-      <c r="I23" s="4" t="n">
-        <v>45482</v>
-      </c>
-      <c r="J23" s="2" t="inlineStr">
-        <is>
-          <t>Núcleo familiar/Responsável primário</t>
-        </is>
-      </c>
-      <c r="K23" s="5" t="inlineStr">
-        <is>
-          <t>- Olá irmãos, por favor informar o nome completo do pai do participante sem estar tudo em letra maiúscula, apenas as letras iniciais de cada nome.</t>
-        </is>
-      </c>
-      <c r="L23" s="2" t="inlineStr">
-        <is>
-          <t>BR0601</t>
-        </is>
-      </c>
-      <c r="M23" s="2" t="inlineStr">
-        <is>
-          <t>Vencida (19-23)</t>
-        </is>
-      </c>
-      <c r="N23" s="2" t="inlineStr">
-        <is>
-          <t>Sponsored</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>Rose Gomes</t>
-        </is>
-      </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>BR060100254</t>
-        </is>
-      </c>
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t>Ana Julia Ribeiro da Silva</t>
-        </is>
-      </c>
-      <c r="D24" s="2" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E24" s="3" t="n">
-        <v>234</v>
-      </c>
-      <c r="F24" s="2" t="inlineStr">
-        <is>
-          <t>3-5</t>
-        </is>
-      </c>
-      <c r="G24" s="2" t="inlineStr">
-        <is>
-          <t>Diana Oliveira</t>
-        </is>
-      </c>
-      <c r="H24" s="4" t="n">
-        <v>44887</v>
-      </c>
-      <c r="I24" s="4" t="n">
-        <v>45146</v>
-      </c>
-      <c r="J24" s="2" t="n"/>
-      <c r="K24" s="5" t="n"/>
-      <c r="L24" s="2" t="inlineStr">
-        <is>
-          <t>BR0601</t>
-        </is>
-      </c>
-      <c r="M24" s="2" t="inlineStr">
-        <is>
-          <t>Vencida (19-23)</t>
-        </is>
-      </c>
-      <c r="N24" s="2" t="inlineStr">
-        <is>
-          <t>Sponsored</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="135" customHeight="1">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>Rose Gomes</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>BR060100322</t>
-        </is>
-      </c>
-      <c r="C25" s="2" t="inlineStr">
-        <is>
-          <t>Arthur Soares Pereira Dinis</t>
-        </is>
-      </c>
-      <c r="D25" s="2" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E25" s="3" t="n">
-        <v>277</v>
-      </c>
-      <c r="F25" s="2" t="inlineStr">
-        <is>
-          <t>6-8</t>
-        </is>
-      </c>
-      <c r="G25" s="2" t="inlineStr">
-        <is>
-          <t>Irisnalda Fernandes da Silva</t>
-        </is>
-      </c>
-      <c r="H25" s="4" t="n">
-        <v>44844</v>
-      </c>
-      <c r="I25" s="4" t="n">
-        <v>45461</v>
-      </c>
-      <c r="J25" s="2" t="inlineStr">
-        <is>
-          <t>Núcleo familiar/Responsável primário; Peso e altura errados/desatualizados</t>
-        </is>
-      </c>
-      <c r="K25" s="5" t="inlineStr">
-        <is>
-          <t>- Olá irmãos, peço que revisem a altura do participante, pois na última atualização consta que ele reduziu, verificar se a altura informada condiz com a realidade, se não, realizar as devidas alterações. - Irmãos, por gentileza corrigir os nomes dos familiares no núcleo familiar sem estar tudo em letra maiúscula.</t>
-        </is>
-      </c>
-      <c r="L25" s="2" t="inlineStr">
-        <is>
-          <t>BR0601</t>
-        </is>
-      </c>
-      <c r="M25" s="2" t="inlineStr">
-        <is>
-          <t>Vencida (19-23)</t>
-        </is>
-      </c>
-      <c r="N25" s="2" t="inlineStr">
-        <is>
-          <t>Sponsored</t>
-        </is>
-      </c>
-    </row>
     <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>Rose Gomes</t>
-        </is>
-      </c>
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>BR060100170</t>
-        </is>
-      </c>
-      <c r="C26" s="2" t="inlineStr">
-        <is>
-          <t>Miguel Nunes Farias</t>
-        </is>
-      </c>
-      <c r="D26" s="2" t="inlineStr">
-        <is>
-          <t>Aprovado</t>
-        </is>
-      </c>
-      <c r="E26" s="3" t="n">
-        <v>252</v>
-      </c>
-      <c r="F26" s="2" t="inlineStr">
-        <is>
-          <t>9-11</t>
-        </is>
-      </c>
-      <c r="G26" s="2" t="inlineStr">
-        <is>
-          <t>Sabrina Martins</t>
-        </is>
-      </c>
-      <c r="H26" s="4" t="n">
-        <v>44869</v>
-      </c>
-      <c r="I26" s="4" t="n">
-        <v>44869</v>
-      </c>
-      <c r="J26" s="2" t="n"/>
-      <c r="K26" s="5" t="n"/>
-      <c r="L26" s="2" t="inlineStr">
-        <is>
-          <t>BR0601</t>
-        </is>
-      </c>
-      <c r="M26" s="2" t="inlineStr">
-        <is>
-          <t>Vencida (19-23)</t>
-        </is>
-      </c>
-      <c r="N26" s="2" t="inlineStr">
-        <is>
-          <t>Unsponsored</t>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>DBOP_08_UPDATES19OUMAIS</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>Rose Gomes</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="inlineStr">
-        <is>
-          <t>BR060100318</t>
-        </is>
-      </c>
-      <c r="C27" s="2" t="inlineStr">
-        <is>
-          <t>Joao Henrique Rodrigues Monteiro</t>
-        </is>
-      </c>
-      <c r="D27" s="2" t="inlineStr">
-        <is>
-          <t>Aprovado</t>
-        </is>
-      </c>
-      <c r="E27" s="3" t="n">
-        <v>277</v>
-      </c>
-      <c r="F27" s="2" t="inlineStr">
-        <is>
-          <t>6-8</t>
-        </is>
-      </c>
-      <c r="G27" s="2" t="inlineStr">
-        <is>
-          <t>Irisnalda Fernandes da Silva</t>
-        </is>
-      </c>
-      <c r="H27" s="4" t="n">
-        <v>44844</v>
-      </c>
-      <c r="I27" s="4" t="n">
-        <v>44844</v>
-      </c>
-      <c r="J27" s="2" t="n"/>
-      <c r="K27" s="5" t="n"/>
-      <c r="L27" s="2" t="inlineStr">
-        <is>
-          <t>BR0601</t>
-        </is>
-      </c>
-      <c r="M27" s="2" t="inlineStr">
-        <is>
-          <t>Vencida (19-23)</t>
-        </is>
-      </c>
-      <c r="N27" s="2" t="inlineStr">
-        <is>
-          <t>Unsponsored</t>
-        </is>
-      </c>
-    </row>
-    <row r="28" ht="135" customHeight="1">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>Rose Gomes</t>
-        </is>
-      </c>
-      <c r="B28" s="2" t="inlineStr">
-        <is>
-          <t>BR060100087</t>
-        </is>
-      </c>
-      <c r="C28" s="2" t="inlineStr">
-        <is>
-          <t>Debora Raquel da Silva Galdino</t>
-        </is>
-      </c>
-      <c r="D28" s="2" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E28" s="3" t="n">
-        <v>245</v>
-      </c>
-      <c r="F28" s="2" t="inlineStr">
-        <is>
-          <t>12-14</t>
-        </is>
-      </c>
-      <c r="G28" s="2" t="inlineStr">
-        <is>
-          <t>Rayla Rodrigues</t>
-        </is>
-      </c>
-      <c r="H28" s="4" t="n">
-        <v>44876</v>
-      </c>
-      <c r="I28" s="4" t="n">
-        <v>45482</v>
-      </c>
-      <c r="J28" s="2" t="inlineStr">
-        <is>
-          <t>Informação Educacional</t>
-        </is>
-      </c>
-      <c r="K28" s="5" t="inlineStr">
-        <is>
-          <t>- Olá irmãos, em 2022 a participante estava cursando o 6° ano do fundamental 2, portanto neste ano de 2024, esperava-se que ela estivesse na 8° série do fundamental 2, peço que revisem para garantir se a informação educacional condiz com a realidade. Em caso de reprovação ou algo similar, explicar através de nota.</t>
-        </is>
-      </c>
-      <c r="L28" s="2" t="inlineStr">
-        <is>
-          <t>BR0601</t>
-        </is>
-      </c>
-      <c r="M28" s="2" t="inlineStr">
-        <is>
-          <t>Vencida (19-23)</t>
-        </is>
-      </c>
-      <c r="N28" s="2" t="inlineStr">
-        <is>
-          <t>Unsponsored</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="45" customHeight="1">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>Rose Gomes</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>BR060100217</t>
-        </is>
-      </c>
-      <c r="C29" s="2" t="inlineStr">
-        <is>
-          <t>Lucas Kaun Fernandes</t>
-        </is>
-      </c>
-      <c r="D29" s="2" t="inlineStr">
-        <is>
-          <t>Devolvido à Igreja Parceira</t>
-        </is>
-      </c>
-      <c r="E29" s="3" t="n">
-        <v>361</v>
-      </c>
-      <c r="F29" s="2" t="inlineStr">
-        <is>
-          <t>6-8</t>
-        </is>
-      </c>
-      <c r="G29" s="2" t="inlineStr">
-        <is>
-          <t>Nayara Oliveira</t>
-        </is>
-      </c>
-      <c r="H29" s="4" t="n">
-        <v>44760</v>
-      </c>
-      <c r="I29" s="4" t="n">
-        <v>45482</v>
-      </c>
-      <c r="J29" s="2" t="inlineStr">
-        <is>
-          <t>Divergência de idade e grupo etário; Núcleo familiar/Responsável primário</t>
-        </is>
-      </c>
-      <c r="K29" s="5" t="inlineStr">
-        <is>
-          <t>Olá irmãos, é necessário que sejam inseridos os nomes completos no núcleo familiar. Atualizar grupo etario.</t>
-        </is>
-      </c>
-      <c r="L29" s="2" t="inlineStr">
-        <is>
-          <t>BR0601</t>
-        </is>
-      </c>
-      <c r="M29" s="2" t="inlineStr">
-        <is>
-          <t>Muito vencida (&gt;=24)</t>
-        </is>
-      </c>
-      <c r="N29" s="2" t="inlineStr">
-        <is>
-          <t>Sponsored</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>DBOP_08_UPDATES19OUMAIS</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Copyright (c) 2000-2024 salesforce.com, inc. Todos os direitos reservados.</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+    <row r="28">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Informações confidenciais - Não distribuir</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Gerado por: BR0601 Administrative / Secretary_Ricardo DanielConserva de Oliveira 13/07/2024 16:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Gerado por: BR0601 Administrative / Secretary_Ricardo DanielConserva de Oliveira 03/08/2024 12:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>Compassion International, Inc.</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N35"/>
+  <autoFilter ref="A1:N30"/>
   <pageMargins left="0.787401575" right="0.787401575" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
 </worksheet>
 </file>
</xml_diff>